<commit_message>
updated engine sheet for epi data extraction
</commit_message>
<xml_diff>
--- a/example_input/std_terms_engine_sheet.xlsx
+++ b/example_input/std_terms_engine_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/ISMS_Work/Project_AIE/Working/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/semiauto-epi-data-extraction-pipeline/example_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BA8BC1-D4DB-F94B-913D-47D5899D890B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F703B2-1303-D947-AFA2-471E9A3B6C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{7D20D1B2-BFFC-5044-9168-1E334BDD6C66}"/>
   </bookViews>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="168">
   <si>
     <t>Project ID</t>
   </si>
@@ -888,13 +888,7 @@
     <t xml:space="preserve">France </t>
   </si>
   <si>
-    <t>Asia</t>
-  </si>
-  <si>
     <t>Prospective</t>
-  </si>
-  <si>
-    <t>White</t>
   </si>
   <si>
     <t>National</t>
@@ -909,13 +903,7 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>North America</t>
-  </si>
-  <si>
     <t>Retrospective</t>
-  </si>
-  <si>
-    <t>Asian</t>
   </si>
   <si>
     <t>Multi-regional</t>
@@ -930,13 +918,7 @@
     <t>Italy</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
     <t>Netither</t>
-  </si>
-  <si>
-    <t>Black or African</t>
   </si>
   <si>
     <t>State/Provincial</t>
@@ -951,12 +933,6 @@
     <t>Spain</t>
   </si>
   <si>
-    <t>South America</t>
-  </si>
-  <si>
-    <t>Hispanic or Latino</t>
-  </si>
-  <si>
     <t>Municipal</t>
   </si>
   <si>
@@ -964,15 +940,6 @@
   </si>
   <si>
     <t>Patient-reported health data</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>Indigenous</t>
   </si>
   <si>
     <t>Facility-level</t>
@@ -984,15 +951,6 @@
     <t>Population health registry</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Middle East and North Africa (MENA)</t>
-  </si>
-  <si>
-    <t>Mixed race</t>
-  </si>
-  <si>
     <t>Cohort study</t>
   </si>
   <si>
@@ -1002,25 +960,10 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>Mutiple ethnic backgrouds</t>
-  </si>
-  <si>
     <t>Medical record review</t>
   </si>
   <si>
-    <t>Latin America and the Caribbean (LAC)</t>
-  </si>
-  <si>
-    <t>Diverse ethnic backgrouds</t>
-  </si>
-  <si>
     <t>Systematic review</t>
-  </si>
-  <si>
-    <t>Oceania (including Australia and Pacific Islands)</t>
   </si>
   <si>
     <t>Genetic epidemiology study</t>
@@ -1036,6 +979,66 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Sub-Saharan Africa</t>
+  </si>
+  <si>
+    <t>Northern Africa and Western Asia</t>
+  </si>
+  <si>
+    <t>Central and Southern Asia</t>
+  </si>
+  <si>
+    <t>Eastern and South-Eastern Asia</t>
+  </si>
+  <si>
+    <t>Latin America and the Caribbean</t>
+  </si>
+  <si>
+    <t>Oceania (excluding Australia and New Zealand)</t>
+  </si>
+  <si>
+    <t>Australia/New Zealand</t>
+  </si>
+  <si>
+    <t>Europe and Northern America</t>
+  </si>
+  <si>
+    <t>Caucasian</t>
+  </si>
+  <si>
+    <t>Jewish</t>
+  </si>
+  <si>
+    <t>Arabs</t>
+  </si>
+  <si>
+    <t>Turks</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>Japanese</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1145,6 +1148,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,13 +1185,126 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1347,120 +1475,7 @@
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1669,19 +1684,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{81AFD4DE-C83B-034F-929A-55E577713CC0}" name="Table3" displayName="Table3" ref="A1:J16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{81AFD4DE-C83B-034F-929A-55E577713CC0}" name="Table3" displayName="Table3" ref="A1:J16" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:J16" xr:uid="{81AFD4DE-C83B-034F-929A-55E577713CC0}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8CF4A79E-24BF-C24B-844D-CC7F41C4D986}" name="Study Population Cohort" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{DCB79477-7A2E-E245-AD2A-B003F5DAA6DA}" name="Disease Phase at Time of Study" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{3790DE9D-48EE-864D-9BBA-FC3FADD3B1EF}" name="Age Groups of Study Cohort" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{10C98258-E10E-A64F-BD32-CF28CC391E24}" name="Study Coverage Area" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{E76953B3-BD62-C94B-95BF-7F78F453016F}" name="Study Design" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{3C3B259F-4726-504F-8D85-9B600F0F74DB}" name="Data Source" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{FE56AB81-7D20-CD40-877D-48252ED4EC9C}" name="Primary Market Focus" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{27B3EF11-BB57-B74D-906F-8FC9D78DA829}" name="Global Region" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{B7158A08-C9C0-C04A-B1C0-80D3DAF256B1}" name="Study Type" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{E4AC3DB8-C47C-184E-A548-11511B6FC262}" name="Primary Ethnicity of Study Cases" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8CF4A79E-24BF-C24B-844D-CC7F41C4D986}" name="Study Population Cohort" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{DCB79477-7A2E-E245-AD2A-B003F5DAA6DA}" name="Disease Phase at Time of Study" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{3790DE9D-48EE-864D-9BBA-FC3FADD3B1EF}" name="Age Groups of Study Cohort" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{10C98258-E10E-A64F-BD32-CF28CC391E24}" name="Study Coverage Area" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{E76953B3-BD62-C94B-95BF-7F78F453016F}" name="Study Design" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3C3B259F-4726-504F-8D85-9B600F0F74DB}" name="Data Source" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{FE56AB81-7D20-CD40-877D-48252ED4EC9C}" name="Primary Market Focus" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{27B3EF11-BB57-B74D-906F-8FC9D78DA829}" name="Global Region" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{B7158A08-C9C0-C04A-B1C0-80D3DAF256B1}" name="Study Type" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{E4AC3DB8-C47C-184E-A548-11511B6FC262}" name="Primary Ethnicity of Study Cases" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2023,7 +2038,7 @@
   <dimension ref="A1:C16384"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51416,12 +51431,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A16384">
-    <cfRule type="beginsWith" dxfId="15" priority="3" operator="beginsWith" text="available">
+    <cfRule type="beginsWith" dxfId="7" priority="3" operator="beginsWith" text="available">
       <formula>LEFT(A1,LEN("available"))="available"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51438,7 +51453,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51737,12 +51752,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A26">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:B16">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51761,10 +51776,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB0D7BF-4E45-1247-BABF-63C8EF6717FB}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51779,10 +51794,11 @@
     <col min="8" max="8" width="40.5" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="11"/>
+    <col min="11" max="11" width="10.83203125" style="11"/>
+    <col min="13" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="9" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
@@ -51801,20 +51817,31 @@
       <c r="F1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="14" t="s">
         <v>44</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>104</v>
       </c>
@@ -51833,20 +51860,30 @@
       <c r="F2" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>118</v>
+      <c r="J2" s="12" t="s">
+        <v>158</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>107</v>
       </c>
@@ -51857,28 +51894,28 @@
         <v>109</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="H3" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>123</v>
+      <c r="J3" s="12" t="s">
+        <v>159</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>110</v>
       </c>
@@ -51889,30 +51926,30 @@
         <v>112</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>128</v>
+      <c r="J4" s="12" t="s">
+        <v>160</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>110</v>
@@ -51921,82 +51958,82 @@
         <v>110</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>137</v>
+      <c r="G5" s="12" t="s">
+        <v>131</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>138</v>
+      <c r="H5" s="15" t="s">
+        <v>153</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>139</v>
+      <c r="J5" s="12" t="s">
+        <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>143</v>
+      <c r="G6" s="13" t="s">
+        <v>148</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>144</v>
+      <c r="H6" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
-      <c r="J6" s="10" t="s">
-        <v>145</v>
+      <c r="J6" s="12" t="s">
+        <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>150</v>
+      <c r="H7" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="10" t="s">
-        <v>151</v>
+      <c r="J7" s="12" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -52004,131 +52041,129 @@
         <v>110</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>154</v>
+      <c r="G8" s="12" t="s">
+        <v>140</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>155</v>
+      <c r="H8" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="10" t="s">
-        <v>156</v>
+      <c r="J8" s="12" t="s">
+        <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>158</v>
+      <c r="H9" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="10" t="s">
-        <v>159</v>
+      <c r="J9" s="12" t="s">
+        <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="F10" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10" t="s">
-        <v>110</v>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="I11" s="10"/>
-      <c r="J11" s="10" t="s">
-        <v>166</v>
+      <c r="J11" s="12" t="s">
+        <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10" t="s">
-        <v>166</v>
-      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -52137,24 +52172,24 @@
         <v>110</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>

</xml_diff>